<commit_message>
Added a ton of validation code to validate the import spreadsheets.
</commit_message>
<xml_diff>
--- a/assets/files/spkrbar-import-template.xlsx
+++ b/assets/files/spkrbar-import-template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>Session Title</t>
   </si>
@@ -44,9 +44,6 @@
     <t>End Time</t>
   </si>
   <si>
-    <t>Time Zone</t>
-  </si>
-  <si>
     <t>Room Name</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>HH:MM AM/PM</t>
   </si>
   <si>
-    <t>EST, PST, etc?</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>http://www.siteone.com, http://www.sitetwo.com</t>
   </si>
   <si>
-    <t>EST</t>
-  </si>
-  <si>
     <t>Windsor Hall</t>
   </si>
   <si>
@@ -215,7 +206,7 @@
     <t>URLs and links need to have “http://” or “www.” at the front, or “.com, .org, etc” at the end.</t>
   </si>
   <si>
-    <t>Please provide as much information as possible. Duplicate information will automatically be filtered out. </t>
+    <t>Please provide as much information as possible. Duplicate information will automatically be filtered out.</t>
   </si>
   <si>
     <t>We do our best to parse nearly every format we can, and it's very rare we encounter things we haven't seen before.</t>
@@ -234,11 +225,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="MM/DD/YY" numFmtId="165"/>
     <numFmt formatCode="HH:MM\ AM/PM" numFmtId="166"/>
-    <numFmt formatCode="HH:MM:SS\ AM/PM" numFmtId="167"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -306,7 +296,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -324,10 +314,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -352,10 +338,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="J1" activeCellId="0" pane="topLeft" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -367,16 +353,16 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.484693877551"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.2908163265306"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0051020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="50.8928571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.6122448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.8877551020408"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.2091836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="37.1326530612245"/>
-    <col collapsed="false" hidden="false" max="257" min="20" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.0051020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="50.8928571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.6122448979592"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.8877551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.2091836734694"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="37.1326530612245"/>
+    <col collapsed="false" hidden="false" max="256" min="19" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.7" outlineLevel="0" r="1">
@@ -413,13 +399,13 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="0" t="s">
@@ -434,146 +420,137 @@
       <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="Q2" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="G5" s="3" t="n">
         <v>41907</v>
@@ -584,153 +561,150 @@
       <c r="I5" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="M5" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="N5" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="O5" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="P5" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="Q5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="R5" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="B8" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="B10" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="B12" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="B13" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="B14" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="B18" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="B19" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="B20" s="0" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="B21" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="B24" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="B25" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="B26" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="B27" s="0" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="http://www.youtube.com/sdkahsld" ref="D5" r:id="rId1"/>
     <hyperlink display="http://www.speakerdeck.com/aksdlkasd" ref="E5" r:id="rId2"/>
-    <hyperlink display="raymond@spkrbar.com" ref="N5" r:id="rId3"/>
-    <hyperlink display="http://www.agilehogs.com" ref="P5" r:id="rId4"/>
-    <hyperlink display="http://www.facebook.com/raymondchandleriii" ref="R5" r:id="rId5"/>
-    <hyperlink display="http://www.linkedin.com/raymond-chandler-iii" ref="S5" r:id="rId6"/>
-    <hyperlink display="https://www.spkrbar.com/manager" ref="B12" r:id="rId7"/>
+    <hyperlink display="raymond@spkrbar.com" ref="M5" r:id="rId3"/>
+    <hyperlink display="http://www.agilehogs.com" ref="O5" r:id="rId4"/>
+    <hyperlink display="http://www.facebook.com/raymondchandleriii" ref="Q5" r:id="rId5"/>
+    <hyperlink display="http://www.linkedin.com/raymond-chandler-iii" ref="R5" r:id="rId6"/>
+    <hyperlink display="5. Visit https://www.spkrbar.com/manager" ref="B12" r:id="rId7"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>